<commit_message>
Added two new Mac-Addresses
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-device_master.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-device_master.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C855F0BA-BDE5-4B60-B365-4E19EAA9D642}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B5B95771-4A63-4BDA-B938-926E8773DD3F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="478">
   <si>
     <t>id</t>
   </si>
@@ -1364,6 +1364,96 @@
   </si>
   <si>
     <t>57-8C-B6-27-5B-18</t>
+  </si>
+  <si>
+    <t>Finger Print Scanner 30</t>
+  </si>
+  <si>
+    <t>IRIS Scanner 30</t>
+  </si>
+  <si>
+    <t>Web Camera 30</t>
+  </si>
+  <si>
+    <t>Document Scanner 30</t>
+  </si>
+  <si>
+    <t>Printer 30</t>
+  </si>
+  <si>
+    <t>D6-15-AC-80-6B-86</t>
+  </si>
+  <si>
+    <t>6D-58-E2-DF-74-34</t>
+  </si>
+  <si>
+    <t>E2-A8-56-86-15-30</t>
+  </si>
+  <si>
+    <t>72-E8-B9-FD-63-65</t>
+  </si>
+  <si>
+    <t>D3-F3-A4-50-AD-12</t>
+  </si>
+  <si>
+    <t>BS563Q2230814</t>
+  </si>
+  <si>
+    <t>BS563Q2230815</t>
+  </si>
+  <si>
+    <t>BS563Q2230816</t>
+  </si>
+  <si>
+    <t>BS563Q2230817</t>
+  </si>
+  <si>
+    <t>BS563Q2230818</t>
+  </si>
+  <si>
+    <t>Finger Print Scanner 31</t>
+  </si>
+  <si>
+    <t>IRIS Scanner 31</t>
+  </si>
+  <si>
+    <t>Web Camera 31</t>
+  </si>
+  <si>
+    <t>Document Scanner 31</t>
+  </si>
+  <si>
+    <t>Printer 31</t>
+  </si>
+  <si>
+    <t>BS563Q2230819</t>
+  </si>
+  <si>
+    <t>BS563Q2230820</t>
+  </si>
+  <si>
+    <t>BS563Q2230821</t>
+  </si>
+  <si>
+    <t>BS563Q2230822</t>
+  </si>
+  <si>
+    <t>BS563Q2230823</t>
+  </si>
+  <si>
+    <t>06-16-D0-0B-A6-E4</t>
+  </si>
+  <si>
+    <t>21-78-45-AC-E9-20</t>
+  </si>
+  <si>
+    <t>3C-E8-87-99-DB-FA</t>
+  </si>
+  <si>
+    <t>BF-55-53-98-40-08</t>
+  </si>
+  <si>
+    <t>5A-43-36-46-22-EB</t>
   </si>
 </sst>
 </file>
@@ -1684,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J146"/>
+  <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5939,8 +6029,298 @@
         <v>212</v>
       </c>
     </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>3000166</v>
+      </c>
+      <c r="B147" t="s">
+        <v>448</v>
+      </c>
+      <c r="C147" t="s">
+        <v>453</v>
+      </c>
+      <c r="D147" t="s">
+        <v>458</v>
+      </c>
+      <c r="F147">
+        <v>165</v>
+      </c>
+      <c r="G147" t="s">
+        <v>210</v>
+      </c>
+      <c r="H147" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I147" t="s">
+        <v>211</v>
+      </c>
+      <c r="J147" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>3000167</v>
+      </c>
+      <c r="B148" t="s">
+        <v>449</v>
+      </c>
+      <c r="C148" t="s">
+        <v>454</v>
+      </c>
+      <c r="D148" t="s">
+        <v>459</v>
+      </c>
+      <c r="F148">
+        <v>327</v>
+      </c>
+      <c r="G148" t="s">
+        <v>210</v>
+      </c>
+      <c r="H148" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I148" t="s">
+        <v>211</v>
+      </c>
+      <c r="J148" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>3000168</v>
+      </c>
+      <c r="B149" t="s">
+        <v>450</v>
+      </c>
+      <c r="C149" t="s">
+        <v>455</v>
+      </c>
+      <c r="D149" t="s">
+        <v>460</v>
+      </c>
+      <c r="F149">
+        <v>736</v>
+      </c>
+      <c r="G149" t="s">
+        <v>210</v>
+      </c>
+      <c r="H149" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I149" t="s">
+        <v>211</v>
+      </c>
+      <c r="J149" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>3000169</v>
+      </c>
+      <c r="B150" t="s">
+        <v>451</v>
+      </c>
+      <c r="C150" t="s">
+        <v>456</v>
+      </c>
+      <c r="D150" t="s">
+        <v>461</v>
+      </c>
+      <c r="F150">
+        <v>801</v>
+      </c>
+      <c r="G150" t="s">
+        <v>210</v>
+      </c>
+      <c r="H150" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I150" t="s">
+        <v>211</v>
+      </c>
+      <c r="J150" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>3000170</v>
+      </c>
+      <c r="B151" t="s">
+        <v>452</v>
+      </c>
+      <c r="C151" t="s">
+        <v>457</v>
+      </c>
+      <c r="D151" t="s">
+        <v>462</v>
+      </c>
+      <c r="F151">
+        <v>920</v>
+      </c>
+      <c r="G151" t="s">
+        <v>210</v>
+      </c>
+      <c r="H151" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I151" t="s">
+        <v>211</v>
+      </c>
+      <c r="J151" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>3000171</v>
+      </c>
+      <c r="B152" t="s">
+        <v>463</v>
+      </c>
+      <c r="C152" t="s">
+        <v>473</v>
+      </c>
+      <c r="D152" t="s">
+        <v>468</v>
+      </c>
+      <c r="F152">
+        <v>165</v>
+      </c>
+      <c r="G152" t="s">
+        <v>210</v>
+      </c>
+      <c r="H152" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I152" t="s">
+        <v>211</v>
+      </c>
+      <c r="J152" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>3000172</v>
+      </c>
+      <c r="B153" t="s">
+        <v>464</v>
+      </c>
+      <c r="C153" t="s">
+        <v>474</v>
+      </c>
+      <c r="D153" t="s">
+        <v>469</v>
+      </c>
+      <c r="F153">
+        <v>327</v>
+      </c>
+      <c r="G153" t="s">
+        <v>210</v>
+      </c>
+      <c r="H153" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I153" t="s">
+        <v>211</v>
+      </c>
+      <c r="J153" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>3000173</v>
+      </c>
+      <c r="B154" t="s">
+        <v>465</v>
+      </c>
+      <c r="C154" t="s">
+        <v>475</v>
+      </c>
+      <c r="D154" t="s">
+        <v>470</v>
+      </c>
+      <c r="F154">
+        <v>736</v>
+      </c>
+      <c r="G154" t="s">
+        <v>210</v>
+      </c>
+      <c r="H154" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I154" t="s">
+        <v>211</v>
+      </c>
+      <c r="J154" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>3000174</v>
+      </c>
+      <c r="B155" t="s">
+        <v>466</v>
+      </c>
+      <c r="C155" t="s">
+        <v>476</v>
+      </c>
+      <c r="D155" t="s">
+        <v>471</v>
+      </c>
+      <c r="F155">
+        <v>801</v>
+      </c>
+      <c r="G155" t="s">
+        <v>210</v>
+      </c>
+      <c r="H155" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I155" t="s">
+        <v>211</v>
+      </c>
+      <c r="J155" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>3000175</v>
+      </c>
+      <c r="B156" t="s">
+        <v>467</v>
+      </c>
+      <c r="C156" t="s">
+        <v>477</v>
+      </c>
+      <c r="D156" t="s">
+        <v>472</v>
+      </c>
+      <c r="F156">
+        <v>920</v>
+      </c>
+      <c r="G156" t="s">
+        <v>210</v>
+      </c>
+      <c r="H156" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I156" t="s">
+        <v>211</v>
+      </c>
+      <c r="J156" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added New Mac-Address and Document Types
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-device_master.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-device_master.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B5B95771-4A63-4BDA-B938-926E8773DD3F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8C019A18-C34A-48B4-BD01-A1E1D639AD49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="493">
   <si>
     <t>id</t>
   </si>
@@ -1454,6 +1454,51 @@
   </si>
   <si>
     <t>5A-43-36-46-22-EB</t>
+  </si>
+  <si>
+    <t>Finger Print Scanner 32</t>
+  </si>
+  <si>
+    <t>IRIS Scanner 32</t>
+  </si>
+  <si>
+    <t>Web Camera 32</t>
+  </si>
+  <si>
+    <t>Document Scanner 32</t>
+  </si>
+  <si>
+    <t>Printer 32</t>
+  </si>
+  <si>
+    <t>80-75-40-E8-CA-24</t>
+  </si>
+  <si>
+    <t>0E-1A-14-4A-6D-3A</t>
+  </si>
+  <si>
+    <t>65-13-7F-0F-F7-53</t>
+  </si>
+  <si>
+    <t>73-C4-DE-8E-C9-8D</t>
+  </si>
+  <si>
+    <t>EC-74-AB-E0-0F-38</t>
+  </si>
+  <si>
+    <t>BS563Q2230824</t>
+  </si>
+  <si>
+    <t>BS563Q2230825</t>
+  </si>
+  <si>
+    <t>BS563Q2230826</t>
+  </si>
+  <si>
+    <t>BS563Q2230827</t>
+  </si>
+  <si>
+    <t>BS563Q2230828</t>
   </si>
 </sst>
 </file>
@@ -1774,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J156"/>
+  <dimension ref="A1:J161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="E156" sqref="E156"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="K113" sqref="K1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6319,6 +6364,151 @@
         <v>212</v>
       </c>
     </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>3000176</v>
+      </c>
+      <c r="B157" t="s">
+        <v>478</v>
+      </c>
+      <c r="C157" t="s">
+        <v>483</v>
+      </c>
+      <c r="D157" t="s">
+        <v>488</v>
+      </c>
+      <c r="F157">
+        <v>165</v>
+      </c>
+      <c r="G157" t="s">
+        <v>210</v>
+      </c>
+      <c r="H157" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I157" t="s">
+        <v>211</v>
+      </c>
+      <c r="J157" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>3000177</v>
+      </c>
+      <c r="B158" t="s">
+        <v>479</v>
+      </c>
+      <c r="C158" t="s">
+        <v>484</v>
+      </c>
+      <c r="D158" t="s">
+        <v>489</v>
+      </c>
+      <c r="F158">
+        <v>327</v>
+      </c>
+      <c r="G158" t="s">
+        <v>210</v>
+      </c>
+      <c r="H158" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I158" t="s">
+        <v>211</v>
+      </c>
+      <c r="J158" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>3000178</v>
+      </c>
+      <c r="B159" t="s">
+        <v>480</v>
+      </c>
+      <c r="C159" t="s">
+        <v>485</v>
+      </c>
+      <c r="D159" t="s">
+        <v>490</v>
+      </c>
+      <c r="F159">
+        <v>736</v>
+      </c>
+      <c r="G159" t="s">
+        <v>210</v>
+      </c>
+      <c r="H159" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I159" t="s">
+        <v>211</v>
+      </c>
+      <c r="J159" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>3000179</v>
+      </c>
+      <c r="B160" t="s">
+        <v>481</v>
+      </c>
+      <c r="C160" t="s">
+        <v>486</v>
+      </c>
+      <c r="D160" t="s">
+        <v>491</v>
+      </c>
+      <c r="F160">
+        <v>801</v>
+      </c>
+      <c r="G160" t="s">
+        <v>210</v>
+      </c>
+      <c r="H160" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I160" t="s">
+        <v>211</v>
+      </c>
+      <c r="J160" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>3000180</v>
+      </c>
+      <c r="B161" t="s">
+        <v>482</v>
+      </c>
+      <c r="C161" t="s">
+        <v>487</v>
+      </c>
+      <c r="D161" t="s">
+        <v>492</v>
+      </c>
+      <c r="F161">
+        <v>920</v>
+      </c>
+      <c r="G161" t="s">
+        <v>210</v>
+      </c>
+      <c r="H161" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I161" t="s">
+        <v>211</v>
+      </c>
+      <c r="J161" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>